<commit_message>
Insert, Delete, Update de la tabla Sucursal
</commit_message>
<xml_diff>
--- a/TP_integrador_Archivos/Informacion_complementaria.xlsx
+++ b/TP_integrador_Archivos/Informacion_complementaria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingunlamedu.sharepoint.com/sites/BasesdeDatosAplicada-Docentes/Documentos compartidos/Docentes/2024/2doCuatrimestre/TP Integrador-Preparacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\OneDrive - Enta Consulting\Escritorio\BBDD Aplicada\TP BBDD Aplicada\TP_integrador_Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{A17665B1-38BF-4AE6-9320-B403BF11F0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2FD1914-B373-4D53-9871-D06CFE300126}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5209B6-2922-4124-9C2A-3EF7F3E83EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{9CB99DF5-F327-421C-B5B9-55DA1B434037}"/>
   </bookViews>
   <sheets>
     <sheet name="sucursal" sheetId="1" r:id="rId1"/>
@@ -1022,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1032,8 +1032,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1330,9 +1329,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1370,7 +1369,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1476,7 +1475,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1618,7 +1617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1632,15 +1631,15 @@
       <selection activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1674,7 +1673,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1724,17 +1723,17 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="76" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -1762,14 +1761,14 @@
       <c r="I2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>257020</v>
       </c>
@@ -1802,7 +1801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>257021</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>257022</v>
       </c>
@@ -1868,7 +1867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>257023</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>257024</v>
       </c>
@@ -1914,7 +1913,7 @@
       <c r="D7">
         <v>30417854</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>239</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1934,7 +1933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>257025</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>257026</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>257027</v>
       </c>
@@ -2033,7 +2032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>257028</v>
       </c>
@@ -2066,7 +2065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>257029</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>257030</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>257031</v>
       </c>
@@ -2165,7 +2164,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>257032</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>257033</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>257034</v>
       </c>
@@ -2244,31 +2243,31 @@
       <c r="D17">
         <v>38974125</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9" t="s">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F21" s="12"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2282,22 +2281,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D68890E-1A4A-4BA5-B83B-61727FCC66D7}">
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>48</v>
       </c>
@@ -2305,7 +2304,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>49</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>50</v>
       </c>
@@ -2330,17 +2329,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932457C5-F4E5-40E2-86CE-923AE54F2BD9}">
   <dimension ref="B1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>34</v>
       </c>
@@ -2356,7 +2355,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>34</v>
       </c>
@@ -2364,7 +2363,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -2372,7 +2371,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>34</v>
       </c>
@@ -2396,7 +2395,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -2404,7 +2403,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>34</v>
       </c>
@@ -2412,7 +2411,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>34</v>
       </c>
@@ -2420,7 +2419,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>37</v>
       </c>
@@ -2436,7 +2435,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>37</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>35</v>
       </c>
@@ -2468,7 +2467,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>38</v>
       </c>
@@ -2484,7 +2483,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -2492,7 +2491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>34</v>
       </c>
@@ -2500,7 +2499,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -2524,7 +2523,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>34</v>
       </c>
@@ -2532,7 +2531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>34</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>37</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>37</v>
       </c>
@@ -2556,7 +2555,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>37</v>
       </c>
@@ -2564,7 +2563,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>34</v>
       </c>
@@ -2572,7 +2571,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>39</v>
       </c>
@@ -2580,7 +2579,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>35</v>
       </c>
@@ -2596,7 +2595,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>34</v>
       </c>
@@ -2604,7 +2603,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>34</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>37</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -2636,7 +2635,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -2644,7 +2643,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>34</v>
       </c>
@@ -2652,7 +2651,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>35</v>
       </c>
@@ -2660,7 +2659,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>35</v>
       </c>
@@ -2668,7 +2667,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>35</v>
       </c>
@@ -2676,7 +2675,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>35</v>
       </c>
@@ -2684,7 +2683,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>40</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>34</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>34</v>
       </c>
@@ -2708,7 +2707,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>37</v>
       </c>
@@ -2716,7 +2715,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>34</v>
       </c>
@@ -2724,7 +2723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>40</v>
       </c>
@@ -2732,7 +2731,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>35</v>
       </c>
@@ -2740,7 +2739,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>41</v>
       </c>
@@ -2748,7 +2747,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>34</v>
       </c>
@@ -2756,7 +2755,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>37</v>
       </c>
@@ -2764,7 +2763,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>37</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>34</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>34</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>42</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>34</v>
       </c>
@@ -2804,7 +2803,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>40</v>
       </c>
@@ -2812,7 +2811,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>34</v>
       </c>
@@ -2820,7 +2819,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>34</v>
       </c>
@@ -2828,7 +2827,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>37</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>34</v>
       </c>
@@ -2844,7 +2843,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>43</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>43</v>
       </c>
@@ -2860,7 +2859,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>40</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>40</v>
       </c>
@@ -2876,7 +2875,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>40</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>34</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>40</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>39</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>34</v>
       </c>
@@ -2916,7 +2915,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>35</v>
       </c>
@@ -2924,7 +2923,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>34</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>37</v>
       </c>
@@ -2940,7 +2939,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>34</v>
       </c>
@@ -2948,7 +2947,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>40</v>
       </c>
@@ -2956,7 +2955,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>39</v>
       </c>
@@ -2964,7 +2963,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>40</v>
       </c>
@@ -2972,7 +2971,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>40</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>40</v>
       </c>
@@ -2988,7 +2987,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>40</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>40</v>
       </c>
@@ -3004,7 +3003,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>40</v>
       </c>
@@ -3012,7 +3011,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>35</v>
       </c>
@@ -3020,7 +3019,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>37</v>
       </c>
@@ -3028,7 +3027,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>37</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>34</v>
       </c>
@@ -3044,7 +3043,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>37</v>
       </c>
@@ -3052,7 +3051,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>34</v>
       </c>
@@ -3060,7 +3059,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>34</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>37</v>
       </c>
@@ -3076,7 +3075,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>41</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>34</v>
       </c>
@@ -3092,7 +3091,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>34</v>
       </c>
@@ -3100,7 +3099,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>34</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>34</v>
       </c>
@@ -3116,7 +3115,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>40</v>
       </c>
@@ -3124,7 +3123,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>41</v>
       </c>
@@ -3132,7 +3131,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>34</v>
       </c>
@@ -3140,7 +3139,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>34</v>
       </c>
@@ -3148,7 +3147,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>34</v>
       </c>
@@ -3156,7 +3155,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>35</v>
       </c>
@@ -3164,7 +3163,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>35</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>42</v>
       </c>
@@ -3180,7 +3179,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>37</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>37</v>
       </c>
@@ -3196,7 +3195,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>37</v>
       </c>
@@ -3204,7 +3203,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>37</v>
       </c>
@@ -3212,7 +3211,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>37</v>
       </c>
@@ -3220,7 +3219,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>34</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>40</v>
       </c>
@@ -3236,7 +3235,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>36</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>34</v>
       </c>
@@ -3252,7 +3251,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>44</v>
       </c>
@@ -3260,7 +3259,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>44</v>
       </c>
@@ -3268,7 +3267,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>34</v>
       </c>
@@ -3276,7 +3275,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>35</v>
       </c>
@@ -3284,7 +3283,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>34</v>
       </c>
@@ -3292,7 +3291,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>34</v>
       </c>
@@ -3300,7 +3299,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>34</v>
       </c>
@@ -3308,7 +3307,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>39</v>
       </c>
@@ -3316,7 +3315,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>39</v>
       </c>
@@ -3324,7 +3323,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>39</v>
       </c>
@@ -3332,7 +3331,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>34</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>39</v>
       </c>
@@ -3348,7 +3347,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>34</v>
       </c>
@@ -3356,7 +3355,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>34</v>
       </c>
@@ -3364,7 +3363,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>34</v>
       </c>
@@ -3372,7 +3371,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>34</v>
       </c>
@@ -3380,7 +3379,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>39</v>
       </c>
@@ -3388,7 +3387,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>35</v>
       </c>
@@ -3396,7 +3395,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>37</v>
       </c>
@@ -3404,7 +3403,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>37</v>
       </c>
@@ -3412,7 +3411,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>39</v>
       </c>
@@ -3420,7 +3419,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>34</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>40</v>
       </c>
@@ -3436,7 +3435,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>37</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>36</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>37</v>
       </c>
@@ -3460,7 +3459,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>39</v>
       </c>
@@ -3468,7 +3467,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>39</v>
       </c>
@@ -3476,7 +3475,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>39</v>
       </c>
@@ -3484,7 +3483,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>39</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>34</v>
       </c>
@@ -3500,7 +3499,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>34</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>34</v>
       </c>
@@ -3516,7 +3515,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>34</v>
       </c>
@@ -3524,7 +3523,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>34</v>
       </c>
@@ -3545,28 +3544,28 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>203</v>
       </c>
@@ -3577,6 +3576,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E0244CD539E758458F9751B276EDBDB5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="940421aca186f6b6cf253ceb76bcb39c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29" xmlns:ns3="5ab81898-6d95-4a49-9528-d5d2a870eede" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4f5da10e60c2eff5832bc3c34d166e5" ns2:_="" ns3:_="">
     <xsd:import namespace="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
@@ -3787,26 +3805,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{664D04EC-A970-41D8-9994-316B682115F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3823,22 +3840,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{652FEED1-E158-4EC5-B971-D1B087C7E1CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E17D9C7C-79F5-4A33-AEBC-02D7C68BFB0C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1a4ef89-8e8d-479e-83ea-6deabd5e5c29"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>